<commit_message>
Retoques en la base de datos
Pequeñas modificaciones en la base de datos para una mejor entrada de datos.
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\OneDrive\Escritorio\CLASE\TFG\HealthApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\eclipse-workspace\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95E86FC9-D696-478F-A25E-F092C5C7D94D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8BB14432-7E61-4A26-9028-904C7D2E99C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{6CF15E38-2B6F-444F-A37E-71752F20310D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -60,85 +60,10 @@
     <t>Calorias</t>
   </si>
   <si>
-    <t>18.90</t>
-  </si>
-  <si>
-    <t>29.3</t>
-  </si>
-  <si>
-    <t>51.3</t>
-  </si>
-  <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>75.9</t>
-  </si>
-  <si>
-    <t>41.6</t>
-  </si>
-  <si>
-    <t>17.5</t>
-  </si>
-  <si>
-    <t>94.5</t>
-  </si>
-  <si>
-    <t>73.4</t>
-  </si>
-  <si>
-    <t>15.8</t>
-  </si>
-  <si>
     <t>Tipo de comida</t>
   </si>
   <si>
-    <t>39.6</t>
-  </si>
-  <si>
-    <t>8.40</t>
-  </si>
-  <si>
-    <t>38.9</t>
-  </si>
-  <si>
-    <t>12.40</t>
-  </si>
-  <si>
     <t>Flan</t>
-  </si>
-  <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>3.10</t>
-  </si>
-  <si>
-    <t>37.4</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>33.3</t>
-  </si>
-  <si>
-    <t>5.6</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>25.3</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>19.6</t>
   </si>
 </sst>
 </file>
@@ -499,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F4022B-8FC8-4575-92D6-64F9DC7D4E1D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +459,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -544,20 +469,20 @@
       <c r="B2">
         <v>547</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="C2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D2">
+        <v>9.4</v>
+      </c>
+      <c r="E2">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="F2">
+        <v>41.6</v>
+      </c>
+      <c r="G2">
+        <v>17.5</v>
       </c>
       <c r="H2">
         <v>15</v>
@@ -570,20 +495,20 @@
       <c r="B3">
         <v>922</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
+      <c r="C3">
+        <v>51.3</v>
+      </c>
+      <c r="D3">
+        <v>29.3</v>
+      </c>
+      <c r="E3">
+        <v>94.5</v>
+      </c>
+      <c r="F3">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="G3">
+        <v>15.8</v>
       </c>
       <c r="H3">
         <v>15</v>
@@ -596,20 +521,20 @@
       <c r="B4">
         <v>566</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
+      <c r="C4">
+        <v>39.6</v>
+      </c>
+      <c r="D4">
+        <v>8.4</v>
+      </c>
+      <c r="E4">
+        <v>38.9</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12.4</v>
       </c>
       <c r="H4">
         <v>15</v>
@@ -617,25 +542,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>244</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
+      <c r="C5">
+        <v>7.4</v>
+      </c>
+      <c r="D5">
+        <v>3.1</v>
+      </c>
+      <c r="E5">
+        <v>37.4</v>
+      </c>
+      <c r="F5">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -648,27 +573,27 @@
       <c r="B6">
         <v>161</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
+      <c r="C6">
+        <v>5.6</v>
+      </c>
+      <c r="D6">
+        <v>3.2</v>
+      </c>
+      <c r="E6">
+        <v>25.3</v>
+      </c>
+      <c r="F6">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.56999999999999995</v>
       </c>
       <c r="H6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" s="1"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
De Openpyxl a Pandas
Se cambia el método de cargar la base de datos de Excel de Openpyxl a Pandas, debido a que mejora la rapidez y sencillez de la carga de datos.
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\eclipse-workspace\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8BB14432-7E61-4A26-9028-904C7D2E99C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43D9212D-1542-439C-BB82-3D1310386EF4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{6CF15E38-2B6F-444F-A37E-71752F20310D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Flan</t>
+  </si>
+  <si>
+    <t>LRE</t>
   </si>
 </sst>
 </file>
@@ -424,19 +427,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F4022B-8FC8-4575-92D6-64F9DC7D4E1D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,8 +465,11 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -487,8 +494,11 @@
       <c r="H2">
         <v>15</v>
       </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -513,8 +523,11 @@
       <c r="H3">
         <v>15</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -539,8 +552,11 @@
       <c r="H4">
         <v>15</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -565,8 +581,11 @@
       <c r="H5">
         <v>15</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -591,8 +610,11 @@
       <c r="H6">
         <v>15</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios muestra de alimentos
Se cambia la forma de indexar los alimentos para que te ofrezca los 3 primeros en la tabla.
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -43,19 +43,19 @@
     <t>LRE</t>
   </si>
   <si>
+    <t>Flan</t>
+  </si>
+  <si>
+    <t>Manzana Asada</t>
+  </si>
+  <si>
     <t>Tarta de queso</t>
   </si>
   <si>
+    <t>Torrijas</t>
+  </si>
+  <si>
     <t>Tarta de chocolate</t>
-  </si>
-  <si>
-    <t>Flan</t>
-  </si>
-  <si>
-    <t>Manzana Asada</t>
-  </si>
-  <si>
-    <t>Torrijas</t>
   </si>
 </sst>
 </file>
@@ -450,28 +450,28 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
-        <v>547</v>
+        <v>244</v>
       </c>
       <c r="D2">
-        <v>18.9</v>
+        <v>7.4</v>
       </c>
       <c r="E2">
-        <v>9.4</v>
+        <v>3.1</v>
       </c>
       <c r="F2">
-        <v>75.90000000000001</v>
+        <v>37.4</v>
       </c>
       <c r="G2">
-        <v>41.6</v>
+        <v>33.3</v>
       </c>
       <c r="H2">
-        <v>17.5</v>
+        <v>7</v>
       </c>
       <c r="I2">
         <v>15</v>
@@ -482,28 +482,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>922</v>
+        <v>161</v>
       </c>
       <c r="D3">
-        <v>51.3</v>
+        <v>5.6</v>
       </c>
       <c r="E3">
-        <v>29.3</v>
+        <v>3.2</v>
       </c>
       <c r="F3">
-        <v>94.5</v>
+        <v>25.3</v>
       </c>
       <c r="G3">
-        <v>73.40000000000001</v>
+        <v>19.6</v>
       </c>
       <c r="H3">
-        <v>15.8</v>
+        <v>0.57</v>
       </c>
       <c r="I3">
         <v>15</v>
@@ -514,98 +514,98 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>244</v>
+        <v>547</v>
       </c>
       <c r="D4">
-        <v>7.4</v>
+        <v>18.9</v>
       </c>
       <c r="E4">
-        <v>3.1</v>
+        <v>9.4</v>
       </c>
       <c r="F4">
-        <v>37.4</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="G4">
-        <v>33.3</v>
+        <v>41.6</v>
       </c>
       <c r="H4">
-        <v>7</v>
+        <v>17.5</v>
       </c>
       <c r="I4">
         <v>15</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
-        <v>161</v>
+        <v>566</v>
       </c>
       <c r="D5">
-        <v>5.6</v>
+        <v>39.6</v>
       </c>
       <c r="E5">
-        <v>3.2</v>
+        <v>8.4</v>
       </c>
       <c r="F5">
-        <v>25.3</v>
+        <v>38.9</v>
       </c>
       <c r="G5">
-        <v>19.6</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>0.57</v>
+        <v>12.4</v>
       </c>
       <c r="I5">
         <v>15</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6">
-        <v>566</v>
+        <v>922</v>
       </c>
       <c r="D6">
-        <v>39.6</v>
+        <v>51.3</v>
       </c>
       <c r="E6">
-        <v>8.4</v>
+        <v>29.3</v>
       </c>
       <c r="F6">
-        <v>38.9</v>
+        <v>94.5</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="H6">
-        <v>12.4</v>
+        <v>15.8</v>
       </c>
       <c r="I6">
         <v>15</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expansion de base de datos
Añadimos nuevos desayunos a la base de daos
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\eclipse-workspace\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B84BD3F-F0C1-4374-8994-047C051638A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFE5323B-83E5-4AC0-9026-ED1D04652BF0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Nombre</t>
   </si>
@@ -45,9 +45,15 @@
     <t>Proteina</t>
   </si>
   <si>
+    <t>Tipo</t>
+  </si>
+  <si>
     <t>LRE</t>
   </si>
   <si>
+    <t>Calidad</t>
+  </si>
+  <si>
     <t>Ensalada de atún</t>
   </si>
   <si>
@@ -57,15 +63,42 @@
     <t>Tarta de chocolate</t>
   </si>
   <si>
+    <t>leche de soja con avena</t>
+  </si>
+  <si>
+    <t>yogurt griego con muesli</t>
+  </si>
+  <si>
+    <t>Leche con cereales</t>
+  </si>
+  <si>
     <t>Torrijas</t>
   </si>
   <si>
+    <t>leche de almendras con avena</t>
+  </si>
+  <si>
+    <t>leche de soja con cereales</t>
+  </si>
+  <si>
     <t>Flan</t>
   </si>
   <si>
+    <t>leche de almendras con cereales</t>
+  </si>
+  <si>
     <t>Manzana Asada</t>
   </si>
   <si>
+    <t>leche de soja con copos de maiz</t>
+  </si>
+  <si>
+    <t>Tortilla francesa(2 huevos)</t>
+  </si>
+  <si>
+    <t>leche con avena</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -78,6 +111,9 @@
     <t>password</t>
   </si>
   <si>
+    <t>sexo</t>
+  </si>
+  <si>
     <t>edad</t>
   </si>
   <si>
@@ -87,6 +123,9 @@
     <t>peso</t>
   </si>
   <si>
+    <t>actividad</t>
+  </si>
+  <si>
     <t>patologia</t>
   </si>
   <si>
@@ -99,18 +138,30 @@
     <t>Guille</t>
   </si>
   <si>
+    <t>Fulano</t>
+  </si>
+  <si>
     <t>carro</t>
   </si>
   <si>
     <t>Calvo</t>
   </si>
   <si>
+    <t>Fulanito</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>nada</t>
   </si>
   <si>
     <t>subir</t>
   </si>
   <si>
+    <t>mantener</t>
+  </si>
+  <si>
     <t>dieta</t>
   </si>
   <si>
@@ -118,18 +169,6 @@
   </si>
   <si>
     <t>bajo azucares</t>
-  </si>
-  <si>
-    <t>sexo</t>
-  </si>
-  <si>
-    <t>actividad</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -531,18 +570,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,18 +601,21 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>383</v>
@@ -602,13 +641,16 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>547</v>
@@ -634,13 +676,16 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>922</v>
@@ -666,101 +711,428 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>386</v>
+      </c>
+      <c r="D5">
+        <v>7.8</v>
+      </c>
+      <c r="E5">
+        <v>1.3</v>
+      </c>
+      <c r="F5">
+        <v>64</v>
+      </c>
+      <c r="G5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H5">
+        <v>15.6</v>
+      </c>
+      <c r="I5">
+        <v>26</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>439</v>
+      </c>
+      <c r="D6">
+        <v>17.2</v>
+      </c>
+      <c r="E6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F6">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="G6">
+        <v>31.4</v>
+      </c>
+      <c r="H6">
+        <v>13.2</v>
+      </c>
+      <c r="I6">
+        <v>31</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>348</v>
+      </c>
+      <c r="D7">
+        <v>13.9</v>
+      </c>
+      <c r="E7">
+        <v>7.6</v>
+      </c>
+      <c r="F7">
+        <v>57.7</v>
+      </c>
+      <c r="G7">
+        <v>25.3</v>
+      </c>
+      <c r="H7">
+        <v>12.7</v>
+      </c>
+      <c r="I7">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>566</v>
+      </c>
+      <c r="D8">
+        <v>39.6</v>
+      </c>
+      <c r="E8">
+        <v>8.4</v>
+      </c>
+      <c r="F8">
+        <v>38.9</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>12.4</v>
+      </c>
+      <c r="I8">
+        <v>31</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>288</v>
+      </c>
+      <c r="D9">
+        <v>6.8</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>46.8</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>11.3</v>
+      </c>
+      <c r="I9">
+        <v>26</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>566</v>
-      </c>
-      <c r="D5">
-        <v>39.6</v>
-      </c>
-      <c r="E5">
-        <v>8.4</v>
-      </c>
-      <c r="F5">
-        <v>38.9</v>
-      </c>
-      <c r="G5">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>353</v>
+      </c>
+      <c r="D10">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E10">
+        <v>3.6</v>
+      </c>
+      <c r="F10">
+        <v>70.3</v>
+      </c>
+      <c r="G10">
+        <v>33.1</v>
+      </c>
+      <c r="H10">
+        <v>10.5</v>
+      </c>
+      <c r="I10">
+        <v>26</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>244</v>
+      </c>
+      <c r="D11">
+        <v>7.4</v>
+      </c>
+      <c r="E11">
+        <v>3.1</v>
+      </c>
+      <c r="F11">
+        <v>37.4</v>
+      </c>
+      <c r="G11">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>255</v>
+      </c>
+      <c r="D12">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E12">
+        <v>3.3</v>
+      </c>
+      <c r="F12">
+        <v>53</v>
+      </c>
+      <c r="G12">
+        <v>21</v>
+      </c>
+      <c r="H12">
+        <v>6.2</v>
+      </c>
+      <c r="I12">
+        <v>26</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>161</v>
+      </c>
+      <c r="D13">
+        <v>5.6</v>
+      </c>
+      <c r="E13">
+        <v>3.2</v>
+      </c>
+      <c r="F13">
+        <v>25.3</v>
+      </c>
+      <c r="G13">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>253</v>
+      </c>
+      <c r="D14">
+        <v>3.8</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="F14">
+        <v>46.4</v>
+      </c>
+      <c r="G14">
+        <v>20.6</v>
+      </c>
+      <c r="H14">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="I14">
+        <v>26</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>385</v>
+      </c>
+      <c r="D15">
+        <v>19.2</v>
+      </c>
+      <c r="E15">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F15">
+        <v>1.6</v>
+      </c>
+      <c r="G15">
+        <v>0.8</v>
+      </c>
+      <c r="H15">
+        <v>26.4</v>
+      </c>
+      <c r="I15">
+        <v>31</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>381</v>
+      </c>
+      <c r="D16">
         <v>12</v>
       </c>
-      <c r="H5">
-        <v>12.4</v>
-      </c>
-      <c r="I5">
-        <v>31</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>244</v>
-      </c>
-      <c r="D6">
-        <v>7.4</v>
-      </c>
-      <c r="E6">
-        <v>3.1</v>
-      </c>
-      <c r="F6">
-        <v>37.4</v>
-      </c>
-      <c r="G6">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>161</v>
-      </c>
-      <c r="D7">
-        <v>5.6</v>
-      </c>
-      <c r="E7">
-        <v>3.2</v>
-      </c>
-      <c r="F7">
-        <v>25.3</v>
-      </c>
-      <c r="G7">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="H7">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="I7">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="E16">
+        <v>5.3</v>
+      </c>
+      <c r="F16">
+        <v>51.5</v>
+      </c>
+      <c r="G16">
+        <v>11.3</v>
+      </c>
+      <c r="H16">
+        <v>17.8</v>
+      </c>
+      <c r="I16">
+        <v>26</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -770,47 +1142,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -821,16 +1191,16 @@
         <v>71308125</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G2">
         <v>24</v>
@@ -845,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -859,16 +1229,16 @@
         <v>1234</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>1234</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G3">
         <v>21</v>
@@ -883,15 +1253,52 @@
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>1234</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>185</v>
+      </c>
+      <c r="I4">
+        <v>83</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -905,13 +1312,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avanzamos en la interfaz
Consigo incluir los frames y cambios de los mismos
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\TFG\HealthApp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A332144E-D78A-45D6-BC17-E0D2617D5011}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
     <sheet name="Usuarios" sheetId="2" r:id="rId2"/>
     <sheet name="Patologias" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -177,8 +171,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,19 +235,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -295,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,27 +313,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,24 +347,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,16 +522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -624,13 +572,13 @@
         <v>547</v>
       </c>
       <c r="D2">
-        <v>18.899999999999999</v>
+        <v>18.9</v>
       </c>
       <c r="E2">
         <v>9.4</v>
       </c>
       <c r="F2">
-        <v>75.900000000000006</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="G2">
         <v>41.6</v>
@@ -648,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -683,7 +631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -703,7 +651,7 @@
         <v>37.4</v>
       </c>
       <c r="G4">
-        <v>33.299999999999997</v>
+        <v>33.3</v>
       </c>
       <c r="H4">
         <v>7</v>
@@ -718,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -738,7 +686,7 @@
         <v>94.5</v>
       </c>
       <c r="G5">
-        <v>73.400000000000006</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="H5">
         <v>15.8</v>
@@ -753,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -788,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -808,10 +756,10 @@
         <v>25.3</v>
       </c>
       <c r="G7">
-        <v>19.600000000000001</v>
+        <v>19.6</v>
       </c>
       <c r="H7">
-        <v>0.56999999999999995</v>
+        <v>0.57</v>
       </c>
       <c r="I7">
         <v>15</v>
@@ -823,7 +771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -858,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -893,7 +841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -916,7 +864,7 @@
         <v>20.6</v>
       </c>
       <c r="H10">
-        <v>77.400000000000006</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="I10">
         <v>26</v>
@@ -928,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -948,7 +896,7 @@
         <v>64</v>
       </c>
       <c r="G11">
-        <v>19.100000000000001</v>
+        <v>19.1</v>
       </c>
       <c r="H11">
         <v>15.6</v>
@@ -963,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -974,7 +922,7 @@
         <v>353</v>
       </c>
       <c r="D12">
-        <v>9.6999999999999993</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E12">
         <v>3.6</v>
@@ -998,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1033,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1044,7 +992,7 @@
         <v>255</v>
       </c>
       <c r="D14">
-        <v>8.6999999999999993</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E14">
         <v>3.3</v>
@@ -1068,7 +1016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1082,10 +1030,10 @@
         <v>17.2</v>
       </c>
       <c r="E15">
-        <v>8.6999999999999993</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F15">
-        <v>71.099999999999994</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="G15">
         <v>31.4</v>
@@ -1103,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1117,7 +1065,7 @@
         <v>19.2</v>
       </c>
       <c r="E16">
-        <v>8.3000000000000007</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F16">
         <v>1.6</v>
@@ -1144,14 +1092,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1186,7 +1134,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1212,7 +1160,7 @@
         <v>178</v>
       </c>
       <c r="I2">
-        <v>73.400000000000006</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="J2">
         <v>4</v>
@@ -1224,7 +1172,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1262,7 +1210,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1306,14 +1254,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1324,7 +1272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1338,7 +1286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Separamos la base de datos
Se separa la base de datos para tratar mejor la información y el guardado de la información del usuario y la de los alimentos
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Desktop\TFG\HealhApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888EC1B-C0D7-44B6-ADFC-A3FE7189D9D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
-    <sheet name="Usuarios" sheetId="2" r:id="rId2"/>
-    <sheet name="Patologias" sheetId="3" r:id="rId3"/>
+    <sheet name="Patologias" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -97,69 +102,6 @@
   </si>
   <si>
     <t>nombre</t>
-  </si>
-  <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>sexo</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>altura</t>
-  </si>
-  <si>
-    <t>peso</t>
-  </si>
-  <si>
-    <t>actividad</t>
-  </si>
-  <si>
-    <t>patologia</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>jesus</t>
-  </si>
-  <si>
-    <t>Guille</t>
-  </si>
-  <si>
-    <t>Ricardo</t>
-  </si>
-  <si>
-    <t>carro</t>
-  </si>
-  <si>
-    <t>Calvo</t>
-  </si>
-  <si>
-    <t>Fernandez</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>subir</t>
-  </si>
-  <si>
-    <t>bajar</t>
   </si>
   <si>
     <t>dieta</t>
@@ -180,8 +122,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,11 +186,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -290,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,9 +272,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,6 +324,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,14 +517,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -578,13 +566,13 @@
         <v>547</v>
       </c>
       <c r="C2">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="D2">
         <v>9.4</v>
       </c>
       <c r="E2">
-        <v>75.90000000000001</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="F2">
         <v>41.6</v>
@@ -602,7 +590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -634,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -651,7 +639,7 @@
         <v>37.4</v>
       </c>
       <c r="F4">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="G4">
         <v>7</v>
@@ -666,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -683,7 +671,7 @@
         <v>94.5</v>
       </c>
       <c r="F5">
-        <v>73.40000000000001</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="G5">
         <v>15.8</v>
@@ -698,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -730,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -747,10 +735,10 @@
         <v>25.3</v>
       </c>
       <c r="F7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G7">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H7">
         <v>15</v>
@@ -762,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -794,7 +782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -826,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -846,7 +834,7 @@
         <v>20.6</v>
       </c>
       <c r="G10">
-        <v>77.40000000000001</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="H10">
         <v>26</v>
@@ -858,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -875,7 +863,7 @@
         <v>64</v>
       </c>
       <c r="F11">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G11">
         <v>15.6</v>
@@ -890,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -898,7 +886,7 @@
         <v>353</v>
       </c>
       <c r="C12">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D12">
         <v>3.6</v>
@@ -922,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -954,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -962,7 +950,7 @@
         <v>255</v>
       </c>
       <c r="C14">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D14">
         <v>3.3</v>
@@ -986,7 +974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -997,10 +985,10 @@
         <v>17.2</v>
       </c>
       <c r="D15">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E15">
-        <v>71.09999999999999</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="F15">
         <v>31.4</v>
@@ -1018,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1029,7 +1017,7 @@
         <v>19.2</v>
       </c>
       <c r="D16">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E16">
         <v>1.6</v>
@@ -1056,14 +1044,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1073,180 +1063,27 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>71308125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2">
-        <v>1234</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2">
-        <v>24</v>
-      </c>
-      <c r="G2">
-        <v>178</v>
-      </c>
-      <c r="H2">
-        <v>73.40000000000001</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>-1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>1234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>1234</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>177</v>
-      </c>
-      <c r="H3">
-        <v>69</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>-1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4">
-        <v>1234</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fallo en editar + incremento base de datos
Se arregla un pequeño fallo en editar, en el cual se seleccionaba solo el desayuno y se amplia la base de datos para hacer pruebas.
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Nombre</t>
   </si>
@@ -90,6 +90,45 @@
   </si>
   <si>
     <t>Tortilla francesa(2 huevos)</t>
+  </si>
+  <si>
+    <t>100 gr arroz + 200 gr filetes pollo empanados + yogurt de chocolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza precocinada mediana </t>
+  </si>
+  <si>
+    <t>100 GR ARROZ + 200 gr pollo frito + manzana</t>
+  </si>
+  <si>
+    <t>150 gr lomo de ternera + 5 croquetas + racion patatas fritas</t>
+  </si>
+  <si>
+    <t>150 gr de pasta + 100 gr lomo de ternera + platano</t>
+  </si>
+  <si>
+    <t>manzana</t>
+  </si>
+  <si>
+    <t>platano</t>
+  </si>
+  <si>
+    <t>tostada de atun (50 gr)</t>
+  </si>
+  <si>
+    <t>yogurt griego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tostada con crema de cacao </t>
+  </si>
+  <si>
+    <t>2 tostadas con creama de cacao</t>
+  </si>
+  <si>
+    <t>150 gr pure de patata + 1 salchicha frankfurt + yogurt</t>
+  </si>
+  <si>
+    <t>150 gramos pure de patata + 100 gramos pollo frito + manzana</t>
   </si>
   <si>
     <t>id</t>
@@ -468,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -529,7 +568,7 @@
         <v>17.5</v>
       </c>
       <c r="H2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -561,7 +600,7 @@
         <v>12.4</v>
       </c>
       <c r="H3">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -593,7 +632,7 @@
         <v>7</v>
       </c>
       <c r="H4">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -625,7 +664,7 @@
         <v>15.8</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -660,7 +699,7 @@
         <v>5</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -689,10 +728,10 @@
         <v>0.57</v>
       </c>
       <c r="H7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -721,7 +760,7 @@
         <v>12.7</v>
       </c>
       <c r="H8">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -753,7 +792,7 @@
         <v>17.8</v>
       </c>
       <c r="H9">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -785,10 +824,10 @@
         <v>77.40000000000001</v>
       </c>
       <c r="H10">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -817,10 +856,10 @@
         <v>15.6</v>
       </c>
       <c r="H11">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -849,7 +888,7 @@
         <v>10.5</v>
       </c>
       <c r="H12">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -881,7 +920,7 @@
         <v>11.3</v>
       </c>
       <c r="H13">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -913,7 +952,7 @@
         <v>6.2</v>
       </c>
       <c r="H14">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -945,10 +984,10 @@
         <v>13.2</v>
       </c>
       <c r="H15">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -977,12 +1016,425 @@
         <v>26.4</v>
       </c>
       <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>1018</v>
+      </c>
+      <c r="C17">
+        <v>37.54</v>
+      </c>
+      <c r="D17">
+        <v>8.51</v>
+      </c>
+      <c r="E17">
+        <v>121.38</v>
+      </c>
+      <c r="F17">
+        <v>8.640000000000001</v>
+      </c>
+      <c r="G17">
+        <v>46.44</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>844</v>
+      </c>
+      <c r="C18">
+        <v>39.2</v>
+      </c>
+      <c r="D18">
+        <v>16.48</v>
+      </c>
+      <c r="E18">
+        <v>88.8</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>32.8</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>689</v>
+      </c>
+      <c r="C19">
+        <v>15.51</v>
+      </c>
+      <c r="D19">
+        <v>2.88</v>
+      </c>
+      <c r="E19">
+        <v>110.74</v>
+      </c>
+      <c r="F19">
+        <v>24.2</v>
+      </c>
+      <c r="G19">
+        <v>24.38</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>821.2</v>
+      </c>
+      <c r="C20">
+        <v>31.066</v>
+      </c>
+      <c r="D20">
+        <v>4.772</v>
+      </c>
+      <c r="E20">
+        <v>82.419</v>
+      </c>
+      <c r="F20">
+        <v>8.085000000000001</v>
+      </c>
+      <c r="G20">
+        <v>51.27399999999999</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>781.5</v>
+      </c>
+      <c r="C21">
+        <v>5.799999999999999</v>
+      </c>
+      <c r="D21">
+        <v>1.465</v>
+      </c>
+      <c r="E21">
+        <v>136.35</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>40.75</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>24</v>
+      </c>
+      <c r="F22">
+        <v>24</v>
+      </c>
+      <c r="G22">
+        <v>0.3</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
+      <c r="B23">
+        <v>140</v>
+      </c>
+      <c r="C23">
+        <v>0.4</v>
+      </c>
+      <c r="D23">
+        <v>0.18</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>1.8</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>242.5</v>
+      </c>
+      <c r="C24">
+        <v>1.54</v>
+      </c>
+      <c r="D24">
+        <v>0.095</v>
+      </c>
+      <c r="E24">
+        <v>48</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>139</v>
+      </c>
+      <c r="C25">
+        <v>10.2</v>
+      </c>
+      <c r="D25">
+        <v>6.8</v>
+      </c>
+      <c r="E25">
+        <v>5.4</v>
+      </c>
+      <c r="F25">
+        <v>5.3</v>
+      </c>
+      <c r="G25">
+        <v>6.4</v>
+      </c>
+      <c r="H25">
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>153.36</v>
+      </c>
+      <c r="C26">
+        <v>5.96</v>
+      </c>
+      <c r="D26">
+        <v>1.864</v>
+      </c>
+      <c r="E26">
+        <v>10.12</v>
+      </c>
+      <c r="F26">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="G26">
+        <v>1.64</v>
+      </c>
+      <c r="H26">
+        <v>26</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>300</v>
+      </c>
+      <c r="C27">
+        <v>11.9</v>
+      </c>
+      <c r="D27">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <v>20.24</v>
+      </c>
+      <c r="F27">
+        <v>19.6</v>
+      </c>
+      <c r="G27">
+        <v>3.28</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1092.84</v>
+      </c>
+      <c r="C28">
+        <v>32.08199999999999</v>
+      </c>
+      <c r="D28">
+        <v>12.147</v>
+      </c>
+      <c r="E28">
+        <v>174.41</v>
+      </c>
+      <c r="F28">
+        <v>51.129</v>
+      </c>
+      <c r="G28">
+        <v>43.664</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>883.5</v>
+      </c>
+      <c r="C29">
+        <v>21.76</v>
+      </c>
+      <c r="D29">
+        <v>2.85</v>
+      </c>
+      <c r="E29">
+        <v>142.94</v>
+      </c>
+      <c r="F29">
+        <v>0.2</v>
+      </c>
+      <c r="G29">
+        <v>24.88</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>1</v>
       </c>
     </row>
@@ -1001,13 +1453,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1015,10 +1467,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1026,10 +1478,10 @@
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadir alimento - FIN
Se termina la función de añadir alimento separada en dos partes, la primera visual, se encuentra en el MAIN, y la segunda, la parte de comprobación y almacenamiento se encuentre en el AdminBase
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\HealthApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E3DF5C-0B94-474C-9EF4-F5B922213A06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
     <sheet name="Patologias" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -155,8 +161,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,11 +225,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -265,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -297,9 +311,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,6 +363,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -506,14 +556,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -553,13 +605,13 @@
         <v>547</v>
       </c>
       <c r="C2">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="D2">
         <v>9.4</v>
       </c>
       <c r="E2">
-        <v>75.90000000000001</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="F2">
         <v>41.6</v>
@@ -577,7 +629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -609,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -626,7 +678,7 @@
         <v>37.4</v>
       </c>
       <c r="F4">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="G4">
         <v>7</v>
@@ -641,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -658,7 +710,7 @@
         <v>94.5</v>
       </c>
       <c r="F5">
-        <v>73.40000000000001</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="G5">
         <v>15.8</v>
@@ -673,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -705,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -722,10 +774,10 @@
         <v>25.3</v>
       </c>
       <c r="F7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G7">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="H7">
         <v>10</v>
@@ -737,7 +789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -769,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -801,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -821,7 +873,7 @@
         <v>20.6</v>
       </c>
       <c r="G10">
-        <v>77.40000000000001</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="H10">
         <v>16</v>
@@ -833,7 +885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -850,7 +902,7 @@
         <v>64</v>
       </c>
       <c r="F11">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G11">
         <v>15.6</v>
@@ -865,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -873,7 +925,7 @@
         <v>353</v>
       </c>
       <c r="C12">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D12">
         <v>3.6</v>
@@ -897,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -929,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -937,7 +989,7 @@
         <v>255</v>
       </c>
       <c r="C14">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D14">
         <v>3.3</v>
@@ -961,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -972,10 +1024,10 @@
         <v>17.2</v>
       </c>
       <c r="D15">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E15">
-        <v>71.09999999999999</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="F15">
         <v>31.4</v>
@@ -993,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1004,7 +1056,7 @@
         <v>19.2</v>
       </c>
       <c r="D16">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E16">
         <v>1.6</v>
@@ -1025,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1042,7 +1094,7 @@
         <v>121.38</v>
       </c>
       <c r="F17">
-        <v>8.640000000000001</v>
+        <v>8.64</v>
       </c>
       <c r="G17">
         <v>46.44</v>
@@ -1057,7 +1109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1065,7 +1117,7 @@
         <v>844</v>
       </c>
       <c r="C18">
-        <v>39.2</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="D18">
         <v>16.48</v>
@@ -1077,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -1089,7 +1141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1121,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1129,19 +1181,19 @@
         <v>821.2</v>
       </c>
       <c r="C20">
-        <v>31.066</v>
+        <v>31.065999999999999</v>
       </c>
       <c r="D20">
-        <v>4.772</v>
+        <v>4.7720000000000002</v>
       </c>
       <c r="E20">
-        <v>82.419</v>
+        <v>82.418999999999997</v>
       </c>
       <c r="F20">
-        <v>8.085000000000001</v>
+        <v>8.0850000000000009</v>
       </c>
       <c r="G20">
-        <v>51.27399999999999</v>
+        <v>51.273999999999987</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -1153,7 +1205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1161,10 +1213,10 @@
         <v>781.5</v>
       </c>
       <c r="C21">
-        <v>5.799999999999999</v>
+        <v>5.7999999999999989</v>
       </c>
       <c r="D21">
-        <v>1.465</v>
+        <v>1.4650000000000001</v>
       </c>
       <c r="E21">
         <v>136.35</v>
@@ -1185,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1217,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1246,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1257,7 +1309,7 @@
         <v>1.54</v>
       </c>
       <c r="D24">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="E24">
         <v>48</v>
@@ -1266,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>8.470000000000001</v>
+        <v>8.4700000000000006</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1278,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1286,7 +1338,7 @@
         <v>139</v>
       </c>
       <c r="C25">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D25">
         <v>6.8</v>
@@ -1310,24 +1362,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
       <c r="B26">
-        <v>153.36</v>
+        <v>153.36000000000001</v>
       </c>
       <c r="C26">
         <v>5.96</v>
       </c>
       <c r="D26">
-        <v>1.864</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="E26">
-        <v>10.12</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="F26">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G26">
         <v>1.64</v>
@@ -1342,7 +1394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1356,10 +1408,10 @@
         <v>2.5</v>
       </c>
       <c r="E27">
-        <v>20.24</v>
+        <v>20.239999999999998</v>
       </c>
       <c r="F27">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G27">
         <v>3.28</v>
@@ -1374,15 +1426,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
       <c r="B28">
-        <v>1092.84</v>
+        <v>1092.8399999999999</v>
       </c>
       <c r="C28">
-        <v>32.08199999999999</v>
+        <v>32.081999999999987</v>
       </c>
       <c r="D28">
         <v>12.147</v>
@@ -1391,10 +1443,10 @@
         <v>174.41</v>
       </c>
       <c r="F28">
-        <v>51.129</v>
+        <v>51.128999999999998</v>
       </c>
       <c r="G28">
-        <v>43.664</v>
+        <v>43.664000000000001</v>
       </c>
       <c r="H28">
         <v>5</v>
@@ -1406,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1444,14 +1496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1462,7 +1514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1473,7 +1525,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1</v>
       </c>

</xml_diff>

<commit_message>
Añadir alimentos v2.0 - Calculo y almacenamiento d
Se calculan los  datos que se insertan de forma gráfica, en base a los gramos insertados en la aplicación. Y se almacenan. Queda pendiente el calculo nutriscore
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E3DF5C-0B94-474C-9EF4-F5B922213A06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9540E-3A43-4859-9D22-C964BDDCF5BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Añadir alimentos - Excepciones
Se arreglan pequeños errores en cuanto al tratamiento de excepciones sobre el metodo añadir alimentos, mas concretamente la comprobación y calculo
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407B9F06-94F5-4AE9-9875-B6398D8F6F58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B4422B-101F-4AE5-8617-FD7D2FB3E087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Añadir menu - Errores
Se arreglan pequeños errores realcionados con el calculo nutriscore y el almacenamiento de datos
</commit_message>
<xml_diff>
--- a/BaseDeDatosDeAlimentos.xlsx
+++ b/BaseDeDatosDeAlimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotace\Desktop\HealthApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCC63C1-97FB-4294-8B1B-A13491AF6127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA725547-2CE0-42B4-9916-7B7160C72B54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimentos" sheetId="1" r:id="rId1"/>
@@ -152,23 +152,23 @@
     <t>dieta</t>
   </si>
   <si>
+    <t>sin patologia</t>
+  </si>
+  <si>
     <t>Diabetes tipo II</t>
   </si>
   <si>
-    <t>sin patologia</t>
+    <t>normal</t>
   </si>
   <si>
     <t>bajo azucares</t>
-  </si>
-  <si>
-    <t>normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,14 +178,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -228,12 +220,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,11 +565,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1686,11 +1680,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1710,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,17 +1713,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>